<commit_message>
modified vue file and raw ontology term xlsx files
</commit_message>
<xml_diff>
--- a/working/ontology terms raw workup.xlsx
+++ b/working/ontology terms raw workup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -265,6 +265,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -286,11 +287,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -347,7 +350,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,14 +376,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,15 +462,15 @@
   </sheetPr>
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B73" activeCellId="0" sqref="B73"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.0204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,11 +618,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -847,8 +842,9 @@
       <c r="B46" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -856,7 +852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -864,7 +860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
@@ -1027,7 +1023,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="7" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>